<commit_message>
added X,Y coords for pupil centers of healthy student images
</commit_message>
<xml_diff>
--- a/data/01_raw/data_h.xlsx
+++ b/data/01_raw/data_h.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\PycharmProjects\radialSegmentation\data\healthy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\PycharmProjects\EyeTraumaAnalysis\data\01_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83D7313-DB90-4182-88B4-DE66A04901FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D0ECB8-6AF7-4CC2-92DF-7418DBA35A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{3CBCD21A-078E-4E09-987F-20379BE29FB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CBCD21A-078E-4E09-987F-20379BE29FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>centerX</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>imageName</t>
-  </si>
-  <si>
-    <t>1_h</t>
   </si>
 </sst>
 </file>
@@ -399,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03771D08-95BF-48FF-8E7C-0D19D9998A03}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,14 +419,135 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>11000</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>196</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>11001</v>
+      </c>
+      <c r="B3">
+        <v>205</v>
+      </c>
+      <c r="C3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>11002</v>
+      </c>
+      <c r="B4">
+        <v>148</v>
+      </c>
+      <c r="C4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>11003</v>
+      </c>
+      <c r="B5">
+        <v>168</v>
+      </c>
+      <c r="C5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>11004</v>
+      </c>
+      <c r="B6">
+        <v>166</v>
+      </c>
+      <c r="C6">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>11005</v>
+      </c>
+      <c r="B7">
+        <v>204</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>11006</v>
+      </c>
+      <c r="B8">
+        <v>135</v>
+      </c>
+      <c r="C8">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>11007</v>
+      </c>
+      <c r="B9">
+        <v>176</v>
+      </c>
+      <c r="C9">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>11008</v>
+      </c>
+      <c r="B10">
+        <v>181</v>
+      </c>
+      <c r="C10">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>11009</v>
+      </c>
+      <c r="B11">
+        <v>158</v>
+      </c>
+      <c r="C11">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11010</v>
+      </c>
+      <c r="B12">
+        <v>183</v>
+      </c>
+      <c r="C12">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>11011</v>
+      </c>
+      <c r="B13">
+        <v>190</v>
+      </c>
+      <c r="C13">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>